<commit_message>
Updated template file for the report
</commit_message>
<xml_diff>
--- a/dist/app/templates/Job Issues Report Template.xlsx
+++ b/dist/app/templates/Job Issues Report Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Documents\Pragmatic\Projects\DBA-Automation-Tools\dist\app\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD4E2910-E985-4C60-8206-1F0B6E431A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16624747-2010-4E1B-9AEC-703BDF04C5C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{B744A78F-2FE8-45D3-96B8-5D845919D6A3}"/>
+    <workbookView xWindow="2610" yWindow="2580" windowWidth="21600" windowHeight="11295" xr2:uid="{B744A78F-2FE8-45D3-96B8-5D845919D6A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">Date - Time </t>
   </si>
@@ -64,11 +64,17 @@
   <si>
     <t>Item Description</t>
   </si>
+  <si>
+    <t>Line #</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -132,11 +138,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -157,6 +160,12 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -492,62 +501,613 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F7CFDEE-D513-43A9-8D63-18A571809A21}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J546"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A3" sqref="A3:XFD546"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12" style="4" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
     </row>
-    <row r="2" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="8"/>
+      <c r="J2" s="7"/>
     </row>
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>